<commit_message>
MODIFY GUOTAI_C ENTRUST DATA IMPORT TEMPLATE
</commit_message>
<xml_diff>
--- a/src/Presentation/CTM.Win/DataTemplate/Entrust/GuoTai_C.xlsx
+++ b/src/Presentation/CTM.Win/DataTemplate/Entrust/GuoTai_C.xlsx
@@ -14,89 +14,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
-  <si>
-    <t>委托日期</t>
-  </si>
-  <si>
-    <t>证券代码</t>
-  </si>
-  <si>
-    <t>证券名称</t>
-  </si>
-  <si>
-    <t>操作</t>
-  </si>
-  <si>
-    <t>委托价格</t>
-  </si>
-  <si>
-    <t>委托数量</t>
-  </si>
-  <si>
-    <t>委托时间</t>
-  </si>
-  <si>
-    <t>成交数量</t>
-  </si>
-  <si>
-    <t>成交均价</t>
-  </si>
-  <si>
-    <t>委托序号</t>
-  </si>
-  <si>
-    <t>交易市场</t>
-  </si>
-  <si>
-    <t>股东帐户</t>
-  </si>
-  <si>
-    <t>备注</t>
-  </si>
-  <si>
-    <t>成交金额</t>
-  </si>
-  <si>
-    <t>帝王洁具</t>
-  </si>
-  <si>
-    <t>普通买入</t>
-  </si>
-  <si>
-    <t>深圳Ａ股</t>
-  </si>
-  <si>
-    <t>部撤</t>
-  </si>
-  <si>
-    <t>普通卖出</t>
-  </si>
-  <si>
-    <t>已成</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>交易类别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>日内</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>波段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>目标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +48,13 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -132,12 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -447,200 +391,243 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
+    <col min="1" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" customWidth="1"/>
+    <col min="13" max="13" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1" t="str">
+        <f>"成交日期"</f>
+        <v>成交日期</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>"成交时间"</f>
+        <v>成交时间</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f>"证券代码"</f>
+        <v>证券代码</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f>"证券名称"</f>
+        <v>证券名称</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f>"买卖标志"</f>
+        <v>买卖标志</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f>"委托价格"</f>
+        <v>委托价格</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f>"委托数量"</f>
+        <v>委托数量</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f>"委托编号"</f>
+        <v>委托编号</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f>"成交价格"</f>
+        <v>成交价格</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f>"成交数量"</f>
+        <v>成交数量</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f>"成交金额"</f>
+        <v>成交金额</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f>"成交编号"</f>
+        <v>成交编号</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f>"股东代码"</f>
+        <v>股东代码</v>
+      </c>
+      <c r="N1" s="1" t="str">
+        <f>"状态说明"</f>
+        <v>状态说明</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
-        <v>20170208</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2798</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1">
-        <v>52.12</v>
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:A4" si="0">"20170809"</f>
+        <v>20170809</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>"09:43:41"</f>
+        <v>09:43:41</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>"002139"</f>
+        <v>002139</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>"拓邦股份"</f>
+        <v>拓邦股份</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>"普通买入"</f>
+        <v>普通买入</v>
       </c>
       <c r="F2" s="1">
-        <v>7700</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.42017361111111112</v>
-      </c>
-      <c r="H2" s="1">
-        <v>6700</v>
+        <v>11.46</v>
+      </c>
+      <c r="G2" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>"22424"</f>
+        <v>22424</v>
       </c>
       <c r="I2" s="1">
-        <v>52.12</v>
+        <v>11.45</v>
       </c>
       <c r="J2" s="1">
-        <v>30678</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="1">
-        <v>604291857</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="1">
-        <v>349204</v>
+        <v>33200</v>
+      </c>
+      <c r="K2" s="1">
+        <v>380140</v>
+      </c>
+      <c r="L2" s="1" t="str">
+        <f>"0103000002122316"</f>
+        <v>0103000002122316</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f t="shared" ref="M2:M4" si="1">"0604291857"</f>
+        <v>0604291857</v>
+      </c>
+      <c r="N2" s="1" t="str">
+        <f t="shared" ref="N2:N4" si="2">"普通成交"</f>
+        <v>普通成交</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>20170208</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2798</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="1">
-        <v>52.65</v>
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>20170809</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>"09:43:41"</f>
+        <v>09:43:41</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>"002139"</f>
+        <v>002139</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>"拓邦股份"</f>
+        <v>拓邦股份</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>"普通买入"</f>
+        <v>普通买入</v>
       </c>
       <c r="F3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.4261921296296296</v>
-      </c>
-      <c r="H3" s="1">
+        <v>11.46</v>
+      </c>
+      <c r="G3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H3" s="1" t="str">
+        <f>"22424"</f>
+        <v>22424</v>
+      </c>
+      <c r="I3" s="1">
+        <v>11.46</v>
+      </c>
+      <c r="J3" s="1">
         <v>200</v>
       </c>
-      <c r="I3" s="1">
-        <v>52.65</v>
-      </c>
-      <c r="J3" s="1">
-        <v>35737</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="1">
-        <v>604291857</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="1">
-        <v>10530</v>
+      <c r="K3" s="1">
+        <v>2292</v>
+      </c>
+      <c r="L3" s="1" t="str">
+        <f>"0103000002122318"</f>
+        <v>0103000002122318</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>0604291857</v>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>普通成交</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>20170208</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2798</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1">
-        <v>52.36</v>
+      <c r="A4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>20170809</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>"09:43:41"</f>
+        <v>09:43:41</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>"002139"</f>
+        <v>002139</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>"拓邦股份"</f>
+        <v>拓邦股份</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f>"普通买入"</f>
+        <v>普通买入</v>
       </c>
       <c r="F4" s="1">
-        <v>12000</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.4303819444444445</v>
-      </c>
-      <c r="H4" s="1">
-        <v>12000</v>
+        <v>11.46</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f>"22424"</f>
+        <v>22424</v>
       </c>
       <c r="I4" s="1">
-        <v>52.36</v>
+        <v>11.46</v>
       </c>
       <c r="J4" s="1">
-        <v>38913</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="1">
-        <v>604291857</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="1">
-        <v>628320</v>
+        <v>500</v>
+      </c>
+      <c r="K4" s="1">
+        <v>5730</v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f>"0103000002122320"</f>
+        <v>0103000002122320</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>0604291857</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>普通成交</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>